<commit_message>
Add handle_excel_data to generate IFC files
</commit_message>
<xml_diff>
--- a/isolants.xlsx
+++ b/isolants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@\@CESI\Stage CESI\Code\Rsimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D929953-F552-4D58-8D90-899C63D5B4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5481F3-BE98-4415-B3AF-F7956620CD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,23 +750,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="15d8ddab-24e7-4977-888d-906390486999" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DC912B4A5A59C479B2BBC606786C189" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="edece333483433262c7d951f9eb38d97">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="15d8ddab-24e7-4977-888d-906390486999" xmlns:ns4="8f3334e0-772c-4b91-a0a5-db773c5e210a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74589bce4edc301c17bb415275c756da" ns3:_="" ns4:_="">
     <xsd:import namespace="15d8ddab-24e7-4977-888d-906390486999"/>
@@ -1013,32 +996,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9035FCF3-51A2-453F-ABDC-26EE19668B74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="15d8ddab-24e7-4977-888d-906390486999"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="8f3334e0-772c-4b91-a0a5-db773c5e210a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27186F30-B619-48AE-8608-D83238E3960A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="15d8ddab-24e7-4977-888d-906390486999" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED63C51F-67DE-4C0B-814F-32585570DF67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1055,4 +1030,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27186F30-B619-48AE-8608-D83238E3960A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9035FCF3-51A2-453F-ABDC-26EE19668B74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="15d8ddab-24e7-4977-888d-906390486999"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="8f3334e0-772c-4b91-a0a5-db773c5e210a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Thickness of Material
</commit_message>
<xml_diff>
--- a/isolants.xlsx
+++ b/isolants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@\@CESI\Stage CESI\Code\Rsimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5481F3-BE98-4415-B3AF-F7956620CD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8351DCAE-4D44-4FBB-B722-636E9B85204C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,6 +750,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="15d8ddab-24e7-4977-888d-906390486999" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DC912B4A5A59C479B2BBC606786C189" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="edece333483433262c7d951f9eb38d97">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="15d8ddab-24e7-4977-888d-906390486999" xmlns:ns4="8f3334e0-772c-4b91-a0a5-db773c5e210a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74589bce4edc301c17bb415275c756da" ns3:_="" ns4:_="">
     <xsd:import namespace="15d8ddab-24e7-4977-888d-906390486999"/>
@@ -996,24 +1013,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27186F30-B619-48AE-8608-D83238E3960A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="15d8ddab-24e7-4977-888d-906390486999" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9035FCF3-51A2-453F-ABDC-26EE19668B74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="15d8ddab-24e7-4977-888d-906390486999"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="8f3334e0-772c-4b91-a0a5-db773c5e210a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED63C51F-67DE-4C0B-814F-32585570DF67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1030,29 +1055,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27186F30-B619-48AE-8608-D83238E3960A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9035FCF3-51A2-453F-ABDC-26EE19668B74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="15d8ddab-24e7-4977-888d-906390486999"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="8f3334e0-772c-4b91-a0a5-db773c5e210a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update IHM to Quickly browse IFC file
</commit_message>
<xml_diff>
--- a/isolants.xlsx
+++ b/isolants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@\@CESI\Stage CESI\Code\Rsimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8351DCAE-4D44-4FBB-B722-636E9B85204C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00691192-8DAD-4489-A4EF-D6D4B6E837E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,23 +750,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="15d8ddab-24e7-4977-888d-906390486999" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DC912B4A5A59C479B2BBC606786C189" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="edece333483433262c7d951f9eb38d97">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="15d8ddab-24e7-4977-888d-906390486999" xmlns:ns4="8f3334e0-772c-4b91-a0a5-db773c5e210a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74589bce4edc301c17bb415275c756da" ns3:_="" ns4:_="">
     <xsd:import namespace="15d8ddab-24e7-4977-888d-906390486999"/>
@@ -1013,10 +996,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="15d8ddab-24e7-4977-888d-906390486999" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27186F30-B619-48AE-8608-D83238E3960A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED63C51F-67DE-4C0B-814F-32585570DF67}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="15d8ddab-24e7-4977-888d-906390486999"/>
+    <ds:schemaRef ds:uri="8f3334e0-772c-4b91-a0a5-db773c5e210a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1039,20 +1050,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED63C51F-67DE-4C0B-814F-32585570DF67}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27186F30-B619-48AE-8608-D83238E3960A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="15d8ddab-24e7-4977-888d-906390486999"/>
-    <ds:schemaRef ds:uri="8f3334e0-772c-4b91-a0a5-db773c5e210a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>